<commit_message>
WebDriverManager Implement, Cross Browser Execution
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/TransitionTestReport.xlsx
+++ b/target/test-classes/TestData/TransitionTestReport.xlsx
@@ -59,14 +59,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" t="s">
+    <row r="2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>